<commit_message>
update dos req funcionais
</commit_message>
<xml_diff>
--- a/Requisitos funcionais/ES2N-Requisitos Funcionais v2.1.xlsx
+++ b/Requisitos funcionais/ES2N-Requisitos Funcionais v2.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ieca\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ieca\OneDrive - GFT Technologies SE\Documents\facul\ES2N_Guaxinim_Raivoso\Requisitos funcionais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2D12FF-7176-49D4-B477-B9A7209F9255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404A4F41-0B59-4FE0-AD42-5A3BE4D96B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t xml:space="preserve">LISTA DE REQUISITOS FUNCIONAIS </t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>RF19</t>
-  </si>
-  <si>
-    <t>Denunciar usuário</t>
   </si>
   <si>
     <t>DATA: 07/04/2022</t>
@@ -236,9 +233,6 @@
     <t>Este requisito permite ao usuário listar todas as tags.</t>
   </si>
   <si>
-    <t>Este requisito permite ao usuário (administrador e gerente de comunidade) criar, alterar, excluir e visualizar comunidades sobre um assunto específico. Todo usuário pode visualizar, criar perguntas e responder dentro de uma comunidade.</t>
-  </si>
-  <si>
     <t>Este requisito permite ao usuário (administrador) criar Tag (palavra-chave) para identificação da categoria da pergunta</t>
   </si>
   <si>
@@ -305,13 +299,28 @@
     <t>Gerenciar posts</t>
   </si>
   <si>
-    <t>Este requisito permite ao usuário (administrador e gerenciador de disciplina) possuir a liberdade de alterar uma pergunta, movê-la de tag, fechá-la e ou associar a outro post duplicado, excluí-la etc.</t>
-  </si>
-  <si>
-    <t>Este requisito permite ao usuário denunciar usuários com comportamento agressivo ou inadequado.</t>
-  </si>
-  <si>
     <t>RF20</t>
+  </si>
+  <si>
+    <t>Este requisito permite ao usuário (administrador e moderador de comunidade) criar, alterar, excluir e visualizar comunidades sobre um assunto específico. Todo usuário pode visualizar, criar perguntas e responder dentro de uma comunidade.</t>
+  </si>
+  <si>
+    <t>Este requisito permite ao usuário (administrador e moderador de disciplina) possuir a liberdade de alterar uma pergunta, movê-la de tag, fechá-la e ou associar a outro post duplicado, excluí-la etc.</t>
+  </si>
+  <si>
+    <t>RF21</t>
+  </si>
+  <si>
+    <t>Gerenciar denúncias</t>
+  </si>
+  <si>
+    <t>O usuário (administrador e moderadores) podem aprovar uma denúncia e bloquear um usuário, ou recusar uma denúncia.</t>
+  </si>
+  <si>
+    <t>Realizar denúncias</t>
+  </si>
+  <si>
+    <t>Este requisito permite ao usuário denunciar usuários com comportamento agressivo ou inadequado em posts e comentários.</t>
   </si>
 </sst>
 </file>
@@ -392,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -407,40 +416,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -759,573 +774,583 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" style="10" customWidth="1"/>
     <col min="3" max="3" width="157.28515625" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="18"/>
+      <c r="A4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="13" t="s">
+      <c r="D18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="69.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="13" t="s">
+    <row r="20" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="69.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="15" t="s">
+      <c r="E24" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="14" t="s">
+    <row r="25" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="26" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="B29" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E29" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-    </row>
     <row r="30" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
     </row>
     <row r="31" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
     </row>
     <row r="33" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
     </row>
     <row r="34" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
     </row>
     <row r="36" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
     </row>
     <row r="37" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
     </row>
     <row r="40" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
     </row>
     <row r="41" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
     </row>
     <row r="42" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
     </row>
     <row r="43" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
     </row>
     <row r="44" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
     </row>
     <row r="45" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
     </row>
     <row r="46" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
     </row>
     <row r="47" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
     </row>
     <row r="48" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
     </row>
     <row r="49" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
     </row>
     <row r="50" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
     </row>
     <row r="51" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
     </row>
     <row r="52" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
     </row>
     <row r="53" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
     </row>
     <row r="54" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
     </row>
     <row r="55" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1337,6 +1362,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010076629F4FB35FC9418E0D886870B51544" ma:contentTypeVersion="4" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7f95b14540eb09806810af4bd4c9fb08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6a6142b7-8324-4fea-855d-77c42805df5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="888c830bd5fcbb6c3d2e267fc73a912e" ns2:_="">
     <xsd:import namespace="6a6142b7-8324-4fea-855d-77c42805df5a"/>
@@ -1480,15 +1514,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1496,6 +1521,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F512524D-8091-4C5A-A973-CA1E8FB50CA2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1509,14 +1542,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add diagramas de caso de uso Alto nível e baixo, update requisitos funcionais, Closes #14
</commit_message>
<xml_diff>
--- a/Requisitos funcionais/ES2N-Requisitos Funcionais v2.1.xlsx
+++ b/Requisitos funcionais/ES2N-Requisitos Funcionais v2.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ieca\OneDrive - GFT Technologies SE\Documents\facul\ES2N_Guaxinim_Raivoso\Requisitos funcionais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404A4F41-0B59-4FE0-AD42-5A3BE4D96B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFD3630-FC80-4D8F-B8C8-7837F5FD4F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1425" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -308,9 +308,6 @@
     <t>Este requisito permite ao usuário (administrador e moderador de disciplina) possuir a liberdade de alterar uma pergunta, movê-la de tag, fechá-la e ou associar a outro post duplicado, excluí-la etc.</t>
   </si>
   <si>
-    <t>RF21</t>
-  </si>
-  <si>
     <t>Gerenciar denúncias</t>
   </si>
   <si>
@@ -321,13 +318,16 @@
   </si>
   <si>
     <t>Este requisito permite ao usuário denunciar usuários com comportamento agressivo ou inadequado em posts e comentários.</t>
+  </si>
+  <si>
+    <t>RF05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,6 +361,12 @@
     </font>
     <font>
       <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,14 +455,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,7 +781,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A10" sqref="A10:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,13 +794,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
@@ -900,7 +906,7 @@
     </row>
     <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>37</v>
@@ -917,7 +923,7 @@
     </row>
     <row r="15" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>39</v>
@@ -934,7 +940,7 @@
     </row>
     <row r="16" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>41</v>
@@ -951,7 +957,7 @@
     </row>
     <row r="17" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>16</v>
@@ -968,9 +974,9 @@
     </row>
     <row r="18" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -983,11 +989,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="69.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="21" t="s">
+    <row r="19" spans="1:5" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -1002,9 +1008,9 @@
     </row>
     <row r="20" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -1019,9 +1025,9 @@
     </row>
     <row r="21" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1036,7 +1042,7 @@
     </row>
     <row r="22" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>24</v>
@@ -1051,9 +1057,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>43</v>
+    <row r="23" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>32</v>
@@ -1069,8 +1075,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
-        <v>44</v>
+      <c r="A24" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>45</v>
@@ -1087,7 +1093,7 @@
     </row>
     <row r="25" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>47</v>
@@ -1104,7 +1110,7 @@
     </row>
     <row r="26" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>49</v>
@@ -1121,13 +1127,13 @@
     </row>
     <row r="27" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>29</v>
@@ -1138,7 +1144,7 @@
     </row>
     <row r="28" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>65</v>
@@ -1155,13 +1161,13 @@
     </row>
     <row r="29" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="C29" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>29</v>
@@ -1356,21 +1362,13 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010076629F4FB35FC9418E0D886870B51544" ma:contentTypeVersion="4" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7f95b14540eb09806810af4bd4c9fb08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6a6142b7-8324-4fea-855d-77c42805df5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="888c830bd5fcbb6c3d2e267fc73a912e" ns2:_="">
     <xsd:import namespace="6a6142b7-8324-4fea-855d-77c42805df5a"/>
@@ -1514,6 +1512,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1521,14 +1528,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F512524D-8091-4C5A-A973-CA1E8FB50CA2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1542,6 +1541,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>